<commit_message>
497550 Uploaded Final Version
</commit_message>
<xml_diff>
--- a/Test/IB_2_0_576 Execution Log.xlsx
+++ b/Test/IB_2_0_576 Execution Log.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="87">
   <si>
     <t>Name</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>IB*2.0*576*T10</t>
-  </si>
-  <si>
     <t>TC289</t>
   </si>
   <si>
@@ -56,9 +53,6 @@
     <t>SQA eBilling TAS US1 Test Case - Date of Onset Printed Regression Test 1 - TS3</t>
   </si>
   <si>
-    <t>IB*2.0*576T10</t>
-  </si>
-  <si>
     <t>TC293</t>
   </si>
   <si>
@@ -173,12 +167,6 @@
     <t>TC224</t>
   </si>
   <si>
-    <t>IB*2.0*576T4</t>
-  </si>
-  <si>
-    <t>IB*2.0*576T5</t>
-  </si>
-  <si>
     <t>TC348</t>
   </si>
   <si>
@@ -221,25 +209,7 @@
     <t>CIT eBilling TAS US1 Test Case - Onset Date - Fatal Error - TS24</t>
   </si>
   <si>
-    <t>IB*2.0*576T6</t>
-  </si>
-  <si>
     <t>Test Case ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IB*2.0*576T5 </t>
-  </si>
-  <si>
-    <t>IB*2.0*576T1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IB*2*576T3 </t>
-  </si>
-  <si>
-    <t>IB*2.0*576T2</t>
-  </si>
-  <si>
-    <t>IB*2.0*576T3</t>
   </si>
   <si>
     <t>SQA eBilling TAS US1 Test Case - Date of Onset Printed Regression Test 2 TS4</t>
@@ -279,16 +249,34 @@
     <t>Not related to current enhancements, Only printing 17 Characters instead of the 18 allowed by the NUCC Guide</t>
   </si>
   <si>
-    <t xml:space="preserve">IB*2.0*576T3 </t>
-  </si>
-  <si>
-    <t>IB*2*576T4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IB*2*576T4 </t>
-  </si>
-  <si>
     <t>DE48 ( Deferred to later build)</t>
+  </si>
+  <si>
+    <t>IB*2.0*576 T1</t>
+  </si>
+  <si>
+    <t>IB*2.0*576 T2</t>
+  </si>
+  <si>
+    <t>IB*2.0*576 T3</t>
+  </si>
+  <si>
+    <t>IB*2.0*576 T5</t>
+  </si>
+  <si>
+    <t>IB*2.0*576 T6</t>
+  </si>
+  <si>
+    <t>IB*2.0*576 T4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IB*2.0*576 T3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IB*2.0*576 T5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IB*2.0*576 T4 </t>
   </si>
 </sst>
 </file>
@@ -944,6 +932,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -961,9 +952,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1309,8 +1297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1327,65 +1315,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="17"/>
+      <c r="A1" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="10" t="s">
         <v>37</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E4" s="6">
         <v>42788</v>
@@ -1394,22 +1382,22 @@
         <v>6</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E5" s="6">
         <v>42795</v>
@@ -1418,22 +1406,22 @@
         <v>6</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E6" s="6">
         <v>42824</v>
@@ -1442,22 +1430,22 @@
         <v>6</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E7" s="6">
         <v>42788</v>
@@ -1466,22 +1454,22 @@
         <v>6</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E8" s="6">
         <v>42795</v>
@@ -1490,22 +1478,22 @@
         <v>6</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E9" s="6">
         <v>42828</v>
@@ -1514,22 +1502,22 @@
         <v>6</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E10" s="6">
         <v>42789</v>
@@ -1538,22 +1526,22 @@
         <v>6</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E11" s="6">
         <v>42795</v>
@@ -1562,22 +1550,22 @@
         <v>6</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E12" s="6">
         <v>42828</v>
@@ -1586,22 +1574,22 @@
         <v>6</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E13" s="6">
         <v>42789</v>
@@ -1610,22 +1598,22 @@
         <v>6</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E14" s="6">
         <v>42795</v>
@@ -1634,22 +1622,22 @@
         <v>6</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="H14" s="12"/>
     </row>
     <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E15" s="6">
         <v>42824</v>
@@ -1658,22 +1646,22 @@
         <v>6</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H15" s="12"/>
     </row>
     <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E16" s="6">
         <v>42789</v>
@@ -1682,22 +1670,22 @@
         <v>6</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="H16" s="12"/>
     </row>
     <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E17" s="6">
         <v>42795</v>
@@ -1706,22 +1694,22 @@
         <v>6</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E18" s="6">
         <v>42828</v>
@@ -1730,22 +1718,22 @@
         <v>6</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E19" s="6">
         <v>42789</v>
@@ -1754,22 +1742,22 @@
         <v>6</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="H19" s="12"/>
     </row>
     <row r="20" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E20" s="6">
         <v>42795</v>
@@ -1778,22 +1766,22 @@
         <v>6</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="H20" s="12"/>
     </row>
     <row r="21" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E21" s="6">
         <v>42828</v>
@@ -1802,22 +1790,22 @@
         <v>6</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H21" s="12"/>
     </row>
     <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E22" s="6">
         <v>42802</v>
@@ -1826,48 +1814,48 @@
         <v>6</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="H22" s="12"/>
     </row>
     <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E23" s="6">
         <v>42816</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E24" s="6">
         <v>42817</v>
@@ -1876,22 +1864,22 @@
         <v>6</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="H24" s="12"/>
     </row>
     <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E25" s="6">
         <v>42824</v>
@@ -1900,22 +1888,22 @@
         <v>6</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H25" s="12"/>
     </row>
     <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E26" s="6">
         <v>42802</v>
@@ -1924,22 +1912,22 @@
         <v>6</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="H26" s="12"/>
     </row>
     <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E27" s="6">
         <v>42824</v>
@@ -1948,22 +1936,22 @@
         <v>6</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H27" s="12"/>
     </row>
     <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E28" s="6">
         <v>42802</v>
@@ -1972,22 +1960,22 @@
         <v>6</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="H28" s="12"/>
     </row>
     <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E29" s="6">
         <v>42825</v>
@@ -1996,22 +1984,22 @@
         <v>6</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H29" s="12"/>
     </row>
     <row r="30" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E30" s="6">
         <v>42802</v>
@@ -2020,22 +2008,22 @@
         <v>6</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="H30" s="12"/>
     </row>
     <row r="31" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E31" s="6">
         <v>42824</v>
@@ -2044,48 +2032,48 @@
         <v>6</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H31" s="12"/>
     </row>
     <row r="32" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E32" s="6">
         <v>42803</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G32" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H32" s="12" t="s">
         <v>74</v>
-      </c>
-      <c r="H32" s="12" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E33" s="6">
         <v>42807</v>
@@ -2094,22 +2082,22 @@
         <v>6</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="H33" s="12"/>
     </row>
     <row r="34" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E34" s="6">
         <v>42828</v>
@@ -2118,22 +2106,22 @@
         <v>6</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H34" s="12"/>
     </row>
     <row r="35" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E35" s="6">
         <v>42807</v>
@@ -2142,22 +2130,22 @@
         <v>6</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="H35" s="12"/>
     </row>
     <row r="36" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E36" s="6">
         <v>42828</v>
@@ -2166,22 +2154,22 @@
         <v>6</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H36" s="12"/>
     </row>
     <row r="37" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E37" s="6">
         <v>42788</v>
@@ -2190,22 +2178,22 @@
         <v>6</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="H37" s="12"/>
     </row>
     <row r="38" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E38" s="6">
         <v>42795</v>
@@ -2214,22 +2202,22 @@
         <v>6</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="H38" s="12"/>
     </row>
     <row r="39" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E39" s="6">
         <v>42802</v>
@@ -2238,22 +2226,22 @@
         <v>6</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="H39" s="12"/>
     </row>
     <row r="40" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E40" s="6">
         <v>42824</v>
@@ -2262,7 +2250,7 @@
         <v>6</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H40" s="12"/>
     </row>
@@ -2286,7 +2274,7 @@
         <v>6</v>
       </c>
       <c r="G41" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="H41" s="12"/>
       <c r="J41" s="8"/>
@@ -2311,16 +2299,16 @@
         <v>6</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H42" s="12"/>
     </row>
     <row r="43" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>4</v>
@@ -2335,16 +2323,16 @@
         <v>6</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H43" s="12"/>
     </row>
     <row r="44" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>4</v>
@@ -2359,16 +2347,16 @@
         <v>6</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H44" s="12"/>
     </row>
     <row r="45" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>4</v>
@@ -2383,16 +2371,16 @@
         <v>6</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H45" s="21"/>
+        <v>84</v>
+      </c>
+      <c r="H45" s="15"/>
     </row>
     <row r="46" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>4</v>
@@ -2407,16 +2395,16 @@
         <v>6</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H46" s="12"/>
     </row>
     <row r="47" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>4</v>
@@ -2431,16 +2419,16 @@
         <v>6</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="H47" s="12"/>
     </row>
     <row r="48" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>4</v>
@@ -2455,16 +2443,16 @@
         <v>6</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H48" s="12"/>
     </row>
     <row r="49" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>4</v>
@@ -2479,16 +2467,16 @@
         <v>6</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H49" s="12"/>
     </row>
     <row r="50" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>4</v>
@@ -2503,16 +2491,16 @@
         <v>6</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H50" s="12"/>
     </row>
     <row r="51" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>4</v>
@@ -2524,21 +2512,21 @@
         <v>42794</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H51" s="12" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>4</v>
@@ -2553,16 +2541,16 @@
         <v>6</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="H52" s="12"/>
     </row>
     <row r="53" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>4</v>
@@ -2577,19 +2565,19 @@
         <v>6</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H53" s="12"/>
     </row>
     <row r="54" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>5</v>
@@ -2598,24 +2586,24 @@
         <v>42816</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G54" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="H54" s="13" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>5</v>
@@ -2624,24 +2612,24 @@
         <v>42817</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="H55" s="13" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>5</v>
@@ -2653,19 +2641,19 @@
         <v>6</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H56" s="12"/>
     </row>
     <row r="57" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>5</v>
@@ -2677,19 +2665,19 @@
         <v>6</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H57" s="12"/>
     </row>
     <row r="58" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>5</v>
@@ -2701,19 +2689,19 @@
         <v>6</v>
       </c>
       <c r="G58" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H58" s="12"/>
     </row>
     <row r="59" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>5</v>
@@ -2725,19 +2713,19 @@
         <v>6</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H59" s="12"/>
     </row>
     <row r="60" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>5</v>
@@ -2749,19 +2737,19 @@
         <v>6</v>
       </c>
       <c r="G60" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="H60" s="12"/>
     </row>
     <row r="61" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>5</v>
@@ -2773,19 +2761,19 @@
         <v>6</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H61" s="12"/>
     </row>
     <row r="62" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A62" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C62" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>5</v>
@@ -2797,19 +2785,19 @@
         <v>6</v>
       </c>
       <c r="G62" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="H62" s="12"/>
     </row>
     <row r="63" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A63" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C63" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>5</v>
@@ -2821,19 +2809,19 @@
         <v>6</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H63" s="12"/>
     </row>
     <row r="64" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A64" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C64" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>5</v>
@@ -2845,19 +2833,19 @@
         <v>6</v>
       </c>
       <c r="G64" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H64"/>
     </row>
     <row r="65" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A65" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C65" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="B65" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>5</v>
@@ -2866,24 +2854,24 @@
         <v>42810</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A66" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C66" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>5</v>
@@ -2895,19 +2883,19 @@
         <v>6</v>
       </c>
       <c r="G66" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="H66" s="12"/>
     </row>
     <row r="67" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A67" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C67" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>5</v>
@@ -2919,19 +2907,19 @@
         <v>6</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H67" s="12"/>
     </row>
     <row r="68" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A68" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>5</v>
@@ -2943,19 +2931,19 @@
         <v>6</v>
       </c>
       <c r="G68" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="H68" s="12"/>
     </row>
     <row r="69" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>5</v>
@@ -2967,16 +2955,16 @@
         <v>6</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H69" s="12"/>
     </row>
     <row r="70" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A70" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>4</v>
@@ -2991,16 +2979,16 @@
         <v>6</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H70" s="12"/>
     </row>
     <row r="71" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A71" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>4</v>
@@ -3015,7 +3003,7 @@
         <v>6</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H71" s="12"/>
     </row>

</xml_diff>